<commit_message>
Guía  didáctica con las recomendaciones realizadas
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/SolicitudGrafica-MA_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/SolicitudGrafica-MA_11_01_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="207">
   <si>
     <t>Fecha:</t>
   </si>
@@ -678,12 +678,6 @@
     <t>Dibujar la union de  intervalos  (-∞,-2)∪(2,∞)  en la recta numérica</t>
   </si>
   <si>
-    <t>Falta llenar de color rojo desde 2 hasta onfinito</t>
-  </si>
-  <si>
-    <t>Necesito que frente a las rectas esten los intervalos, ademas emplear  el simbolo de union</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -694,12 +688,6 @@
   </si>
   <si>
     <t>ok</t>
-  </si>
-  <si>
-    <t>Escribir los intervalos frente a  cada recta numérica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escribir los intervalos frente a  cada recta numérica. </t>
   </si>
   <si>
     <t>Es  necesario utilizar la simbologia matematica, el simbolo de pertenece, la equis en minuscula y  cursiva;  la R caracteristica del conjunto de los numeros reales.</t>
@@ -913,7 +901,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,6 +951,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1508,7 +1502,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1743,12 +1737,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1762,6 +1750,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1845,6 +1845,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -3551,8 +3554,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3590,14 +3593,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="105"/>
-      <c r="F2" s="97" t="s">
+      <c r="D2" s="107"/>
+      <c r="F2" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="98"/>
+      <c r="G2" s="100"/>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
       <c r="J2" s="16"/>
@@ -3607,12 +3610,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="106">
+      <c r="C3" s="108">
         <v>11</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="100"/>
+      <c r="D3" s="109"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="102"/>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
       <c r="J3" s="16"/>
@@ -3622,10 +3625,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="107"/>
+      <c r="D4" s="109"/>
       <c r="E4" s="5"/>
       <c r="F4" s="50" t="s">
         <v>55</v>
@@ -3643,10 +3646,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="110" t="s">
         <v>163</v>
       </c>
-      <c r="D5" s="109"/>
+      <c r="D5" s="111"/>
       <c r="E5" s="5"/>
       <c r="F5" s="48" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -3697,12 +3700,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="101" t="s">
+      <c r="F8" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="103"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="105"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -3784,7 +3787,7 @@
         <v>166</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="12" customFormat="1" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3821,8 +3824,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="14"/>
-      <c r="K11" s="96" t="s">
-        <v>204</v>
+      <c r="K11" s="94" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.25">
@@ -3859,8 +3862,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="77"/>
-      <c r="K12" s="93" t="s">
-        <v>210</v>
+      <c r="K12" s="91" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3897,8 +3900,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13"/>
-      <c r="K13" s="93" t="s">
-        <v>210</v>
+      <c r="K13" s="91" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3934,8 +3937,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="77"/>
-      <c r="K14" s="93" t="s">
-        <v>210</v>
+      <c r="K14" s="91" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -3971,8 +3974,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15"/>
-      <c r="K15" s="93" t="s">
-        <v>210</v>
+      <c r="K15" s="130" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4009,7 +4012,7 @@
       </c>
       <c r="J16" s="77"/>
       <c r="K16" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" ht="255" customHeight="1" x14ac:dyDescent="0.25">
@@ -4045,8 +4048,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="30"/>
-      <c r="K17" s="95" t="s">
-        <v>205</v>
+      <c r="K17" s="93" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="147.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4082,8 +4085,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="77"/>
-      <c r="K18" s="94" t="s">
-        <v>209</v>
+      <c r="K18" s="96" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" ht="183" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4119,8 +4122,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19"/>
-      <c r="K19" s="94" t="s">
-        <v>209</v>
+      <c r="K19" s="96" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4156,8 +4159,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20"/>
-      <c r="K20" s="94" t="s">
-        <v>209</v>
+      <c r="K20" s="96" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
@@ -4193,8 +4196,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J21" s="77"/>
-      <c r="K21" s="94" t="s">
-        <v>209</v>
+      <c r="K21" s="96" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4230,8 +4233,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22"/>
-      <c r="K22" s="94" t="s">
-        <v>209</v>
+      <c r="K22" s="92" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="12" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4267,8 +4270,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="77"/>
-      <c r="K23" s="94" t="s">
-        <v>209</v>
+      <c r="K23" s="96" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4304,8 +4307,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J24"/>
-      <c r="K24" s="94" t="s">
-        <v>209</v>
+      <c r="K24" s="96" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4341,11 +4344,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="77"/>
-      <c r="K25" s="94" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="K25" s="96" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>177</v>
       </c>
@@ -4380,8 +4383,8 @@
       <c r="J26" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="K26" s="93" t="s">
-        <v>207</v>
+      <c r="K26" s="95" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
@@ -4419,8 +4422,8 @@
       <c r="J27" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="K27" s="93" t="s">
-        <v>207</v>
+      <c r="K27" s="95" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4458,11 +4461,11 @@
       <c r="J28" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="K28" s="93" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="K28" s="95" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>184</v>
       </c>
@@ -4497,8 +4500,8 @@
       <c r="J29" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="K29" s="93" t="s">
-        <v>208</v>
+      <c r="K29" s="95" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4537,7 +4540,7 @@
         <v>195</v>
       </c>
       <c r="K30" s="83" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="12" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4576,7 +4579,7 @@
         <v>197</v>
       </c>
       <c r="K31" s="83" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="12" customFormat="1" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4612,8 +4615,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J32"/>
-      <c r="K32" s="92" t="s">
-        <v>204</v>
+      <c r="K32" s="90" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="12" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4652,7 +4655,7 @@
         <v>198</v>
       </c>
       <c r="K33" s="83" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="12" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.25">
@@ -4688,11 +4691,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J34" s="77"/>
-      <c r="K34" s="91" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="K34" s="97" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>199</v>
       </c>
@@ -4727,8 +4730,8 @@
       <c r="J35" s="88" t="s">
         <v>200</v>
       </c>
-      <c r="K35" s="90" t="s">
-        <v>201</v>
+      <c r="K35" s="98" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="12" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7049,25 +7052,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="116"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="42"/>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="117"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="119"/>
       <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -7075,11 +7078,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="42"/>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="123"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="125"/>
       <c r="F3" s="43"/>
       <c r="H3" s="33" t="s">
         <v>18</v>
@@ -7130,11 +7133,11 @@
       <c r="C5" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="124" t="str">
+      <c r="D5" s="126" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>MA_11_01_CO</v>
       </c>
-      <c r="E5" s="125"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="43"/>
       <c r="H5" s="33" t="s">
         <v>22</v>
@@ -7179,12 +7182,12 @@
       <c r="C7" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="110" t="str">
+      <c r="D7" s="112" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_MA_11_01_CO.xls</v>
       </c>
-      <c r="E7" s="110"/>
-      <c r="F7" s="111"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
       <c r="H7" s="33" t="s">
         <v>24</v>
       </c>
@@ -7278,14 +7281,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="114"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="116"/>
       <c r="I13" s="33" t="s">
         <v>33</v>
       </c>
@@ -7318,12 +7321,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="42"/>
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="117"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="119"/>
       <c r="J15" s="33">
         <v>12</v>
       </c>
@@ -7363,12 +7366,12 @@
       <c r="C17" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="118" t="str">
+      <c r="D17" s="120" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>MA_11_01_REC10</v>
       </c>
-      <c r="E17" s="119"/>
-      <c r="F17" s="120"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="122"/>
       <c r="J17" s="33">
         <v>14</v>
       </c>
@@ -7384,12 +7387,12 @@
       <c r="C18" s="73" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="110" t="str">
+      <c r="D18" s="112" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_MA_11_01_REC10.xls</v>
       </c>
-      <c r="E18" s="110"/>
-      <c r="F18" s="111"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="113"/>
       <c r="J18" s="33">
         <v>15</v>
       </c>
@@ -7781,41 +7784,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="126" t="s">
+      <c r="C1" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="126" t="s">
+      <c r="E1" s="128" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="126" t="s">
+      <c r="F1" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="126" t="s">
+      <c r="G1" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="127" t="s">
+      <c r="H1" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
+      <c r="A2" s="128"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
       <c r="H2" s="52" t="s">
         <v>65</v>
       </c>

</xml_diff>